<commit_message>
Minor tweak to datatype
</commit_message>
<xml_diff>
--- a/WaDE_DET_v0.3_Oct2017.xlsx
+++ b/WaDE_DET_v0.3_Oct2017.xlsx
@@ -4585,7 +4585,9 @@
   </sheetPr>
   <dimension ref="A1:L356"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A316" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="D351" sqref="D351:G353"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6469,10 +6471,10 @@
         <v>1290</v>
       </c>
       <c r="D58" s="61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E58" s="65" t="s">
-        <v>207</v>
+        <v>330</v>
       </c>
       <c r="F58" s="59" t="s">
         <v>342</v>
@@ -6513,7 +6515,7 @@
         <v>342</v>
       </c>
       <c r="G59" s="59" t="s">
-        <v>342</v>
+        <v>296</v>
       </c>
       <c r="H59" s="64" t="s">
         <v>1287</v>
@@ -6939,10 +6941,10 @@
         <v>1290</v>
       </c>
       <c r="D72" s="61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E72" s="65" t="s">
-        <v>207</v>
+        <v>330</v>
       </c>
       <c r="F72" s="59" t="s">
         <v>342</v>
@@ -6983,7 +6985,7 @@
         <v>342</v>
       </c>
       <c r="G73" s="59" t="s">
-        <v>342</v>
+        <v>296</v>
       </c>
       <c r="H73" s="64" t="s">
         <v>1287</v>
@@ -8358,10 +8360,10 @@
         <v>1290</v>
       </c>
       <c r="D115" s="61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E115" s="65" t="s">
-        <v>207</v>
+        <v>330</v>
       </c>
       <c r="F115" s="59" t="s">
         <v>342</v>
@@ -8402,7 +8404,7 @@
         <v>342</v>
       </c>
       <c r="G116" s="59" t="s">
-        <v>342</v>
+        <v>296</v>
       </c>
       <c r="H116" s="64" t="s">
         <v>1287</v>
@@ -8887,10 +8889,10 @@
         <v>1290</v>
       </c>
       <c r="D131" s="61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E131" s="65" t="s">
-        <v>207</v>
+        <v>330</v>
       </c>
       <c r="F131" s="59" t="s">
         <v>342</v>
@@ -8931,7 +8933,7 @@
         <v>342</v>
       </c>
       <c r="G132" s="59" t="s">
-        <v>342</v>
+        <v>296</v>
       </c>
       <c r="H132" s="64" t="s">
         <v>1287</v>
@@ -10919,10 +10921,10 @@
         <v>1290</v>
       </c>
       <c r="D193" s="61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E193" s="65" t="s">
-        <v>207</v>
+        <v>330</v>
       </c>
       <c r="F193" s="59" t="s">
         <v>342</v>
@@ -10963,7 +10965,7 @@
         <v>342</v>
       </c>
       <c r="G194" s="59" t="s">
-        <v>342</v>
+        <v>296</v>
       </c>
       <c r="H194" s="64" t="s">
         <v>1287</v>
@@ -11255,10 +11257,10 @@
         <v>1290</v>
       </c>
       <c r="D203" s="61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E203" s="65" t="s">
-        <v>207</v>
+        <v>330</v>
       </c>
       <c r="F203" s="59" t="s">
         <v>342</v>
@@ -11299,7 +11301,7 @@
         <v>342</v>
       </c>
       <c r="G204" s="59" t="s">
-        <v>342</v>
+        <v>296</v>
       </c>
       <c r="H204" s="64" t="s">
         <v>1287</v>
@@ -12870,10 +12872,10 @@
         <v>1290</v>
       </c>
       <c r="D252" s="61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E252" s="65" t="s">
-        <v>207</v>
+        <v>330</v>
       </c>
       <c r="F252" s="59" t="s">
         <v>342</v>
@@ -12914,7 +12916,7 @@
         <v>342</v>
       </c>
       <c r="G253" s="59" t="s">
-        <v>342</v>
+        <v>296</v>
       </c>
       <c r="H253" s="64" t="s">
         <v>1287</v>
@@ -13206,10 +13208,10 @@
         <v>1290</v>
       </c>
       <c r="D262" s="61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E262" s="65" t="s">
-        <v>207</v>
+        <v>330</v>
       </c>
       <c r="F262" s="59" t="s">
         <v>342</v>
@@ -13250,7 +13252,7 @@
         <v>342</v>
       </c>
       <c r="G263" s="59" t="s">
-        <v>342</v>
+        <v>296</v>
       </c>
       <c r="H263" s="64" t="s">
         <v>1287</v>
@@ -14786,10 +14788,10 @@
         <v>1290</v>
       </c>
       <c r="D310" s="61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E310" s="65" t="s">
-        <v>207</v>
+        <v>330</v>
       </c>
       <c r="F310" s="59" t="s">
         <v>342</v>
@@ -14830,7 +14832,7 @@
         <v>342</v>
       </c>
       <c r="G311" s="59" t="s">
-        <v>342</v>
+        <v>296</v>
       </c>
       <c r="H311" s="64" t="s">
         <v>1287</v>
@@ -15846,10 +15848,10 @@
         <v>1290</v>
       </c>
       <c r="D342" s="61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E342" s="65" t="s">
-        <v>207</v>
+        <v>330</v>
       </c>
       <c r="F342" s="59" t="s">
         <v>342</v>
@@ -15890,7 +15892,7 @@
         <v>342</v>
       </c>
       <c r="G343" s="59" t="s">
-        <v>342</v>
+        <v>296</v>
       </c>
       <c r="H343" s="64" t="s">
         <v>1287</v>
@@ -16186,10 +16188,10 @@
         <v>1290</v>
       </c>
       <c r="D352" s="61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E352" s="65" t="s">
-        <v>207</v>
+        <v>330</v>
       </c>
       <c r="F352" s="59" t="s">
         <v>342</v>
@@ -16230,7 +16232,7 @@
         <v>342</v>
       </c>
       <c r="G353" s="59" t="s">
-        <v>342</v>
+        <v>296</v>
       </c>
       <c r="H353" s="64" t="s">
         <v>1287</v>

</xml_diff>